<commit_message>
Update Pendulum Project Verification Matrix.xlsx
</commit_message>
<xml_diff>
--- a/Media/Verification Matrix/Pendulum Project Verification Matrix.xlsx
+++ b/Media/Verification Matrix/Pendulum Project Verification Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbear\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbear\OneDrive\Desktop\Pendulum Project\EG-310-InvertedPendulum\Media\Verification Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BF7330-E98F-42A8-B1E7-71180D161C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD9A384-30E3-45E9-BA3E-79FB460374BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{6297B829-7CF2-4E53-A761-CB565844B553}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6297B829-7CF2-4E53-A761-CB565844B553}"/>
   </bookViews>
   <sheets>
     <sheet name="Ver_Matrix" sheetId="1" r:id="rId1"/>
@@ -961,6 +961,63 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -985,24 +1042,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1024,45 +1063,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1382,304 +1382,304 @@
   </sheetPr>
   <dimension ref="B1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="22" width="4.7109375" customWidth="1"/>
-    <col min="23" max="23" width="4.5703125" customWidth="1"/>
-    <col min="24" max="24" width="4.7109375" customWidth="1"/>
-    <col min="25" max="25" width="4.28515625" customWidth="1"/>
-    <col min="26" max="26" width="36.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="4" width="4.6640625" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" customWidth="1"/>
+    <col min="6" max="22" width="4.6640625" customWidth="1"/>
+    <col min="23" max="23" width="4.5546875" customWidth="1"/>
+    <col min="24" max="24" width="4.6640625" customWidth="1"/>
+    <col min="25" max="25" width="4.33203125" customWidth="1"/>
+    <col min="26" max="26" width="36.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C1" s="49" t="s">
+    <row r="1" spans="2:26" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-    </row>
-    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+    </row>
+    <row r="2" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50" t="s">
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50" t="s">
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50" t="s">
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="50"/>
+      <c r="Y2" s="38"/>
       <c r="Z2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:26" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+    <row r="3" spans="2:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="31" t="s">
+      <c r="L3" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="M3" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="O3" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="P3" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="Q3" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="R3" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="S3" s="46" t="s">
+      <c r="S3" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="31" t="s">
+      <c r="T3" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="U3" s="28" t="s">
+      <c r="U3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="43" t="s">
+      <c r="V3" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="W3" s="31" t="s">
+      <c r="W3" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="X3" s="28" t="s">
+      <c r="X3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" s="31" t="s">
+      <c r="Y3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="Z3" s="34" t="s">
+      <c r="Z3" s="47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="51"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="44"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="35"/>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B5" s="51"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="47"/>
-      <c r="S5" s="47"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="32"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="35"/>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="51"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="44"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="35"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="51"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
-      <c r="S7" s="47"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="44"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="35"/>
-    </row>
-    <row r="8" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="51"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="33"/>
-      <c r="X8" s="30"/>
-      <c r="Y8" s="33"/>
-      <c r="Z8" s="36"/>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B4" s="24"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="48"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B5" s="24"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="48"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B6" s="24"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="48"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B7" s="24"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="48"/>
+    </row>
+    <row r="8" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="24"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="49"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1708,7 @@
       <c r="Y9" s="19"/>
       <c r="Z9" s="4"/>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>29</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
         <v>49</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>50</v>
       </c>
@@ -1865,7 +1865,7 @@
       <c r="V13" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="W13" s="17" t="s">
+      <c r="W13" s="16" t="s">
         <v>74</v>
       </c>
       <c r="X13" s="15"/>
@@ -1874,7 +1874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
         <v>51</v>
       </c>
@@ -1886,7 +1886,7 @@
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="16" t="s">
         <v>76</v>
       </c>
       <c r="L14" s="15"/>
@@ -1902,7 +1902,7 @@
       <c r="V14" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="W14" s="17" t="s">
+      <c r="W14" s="16" t="s">
         <v>84</v>
       </c>
       <c r="X14" s="15"/>
@@ -1911,13 +1911,13 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>76</v>
       </c>
       <c r="F15" s="15"/>
@@ -1926,7 +1926,7 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
-      <c r="L15" s="55" t="s">
+      <c r="L15" s="20" t="s">
         <v>79</v>
       </c>
       <c r="M15" s="15"/>
@@ -1941,7 +1941,7 @@
       <c r="V15" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="W15" s="17" t="s">
+      <c r="W15" s="16" t="s">
         <v>84</v>
       </c>
       <c r="X15" s="15"/>
@@ -1950,7 +1950,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>2</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
         <v>44</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
         <v>33</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
         <v>47</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
         <v>46</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
         <v>48</v>
       </c>
@@ -2147,7 +2147,7 @@
       <c r="D21" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="16" t="s">
         <v>83</v>
       </c>
       <c r="F21" s="17" t="s">
@@ -2186,7 +2186,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>3</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
         <v>30</v>
       </c>
@@ -2225,7 +2225,7 @@
       <c r="D23" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="16" t="s">
         <v>74</v>
       </c>
       <c r="F23" s="17" t="s">
@@ -2237,7 +2237,7 @@
       <c r="J23" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="K23" s="17" t="s">
+      <c r="K23" s="16" t="s">
         <v>74</v>
       </c>
       <c r="L23" s="15"/>
@@ -2255,7 +2255,7 @@
       <c r="V23" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="W23" s="17" t="s">
+      <c r="W23" s="16" t="s">
         <v>84</v>
       </c>
       <c r="X23" s="15"/>
@@ -2264,7 +2264,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B24" s="12" t="s">
         <v>31</v>
       </c>
@@ -2286,7 +2286,7 @@
       <c r="J24" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="K24" s="17" t="s">
+      <c r="K24" s="16" t="s">
         <v>74</v>
       </c>
       <c r="L24" s="15"/>
@@ -2311,13 +2311,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B25" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="16" t="s">
         <v>74</v>
       </c>
       <c r="F25" s="15"/>
@@ -2343,7 +2343,7 @@
       <c r="V25" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="W25" s="17" t="s">
+      <c r="W25" s="16" t="s">
         <v>78</v>
       </c>
       <c r="X25" s="15"/>
@@ -2352,7 +2352,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B26" s="12" t="s">
         <v>34</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B27" s="12" t="s">
         <v>35</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
         <v>36</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B29" s="12" t="s">
         <v>37</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B30" s="12" t="s">
         <v>38</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
         <v>39</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="s">
         <v>40</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B33" s="12" t="s">
         <v>41</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B34" s="12" t="s">
         <v>42</v>
       </c>
@@ -2679,7 +2679,7 @@
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="16" t="s">
         <v>74</v>
       </c>
       <c r="I34" s="15"/>
@@ -2707,14 +2707,14 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B35" s="12" t="s">
         <v>43</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="16" t="s">
         <v>76</v>
       </c>
       <c r="G35" s="15"/>
@@ -2739,7 +2739,7 @@
       <c r="V35" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="W35" s="17" t="s">
+      <c r="W35" s="16" t="s">
         <v>83</v>
       </c>
       <c r="X35" s="15"/>
@@ -2748,7 +2748,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B36" s="12" t="s">
         <v>45</v>
       </c>
@@ -2780,7 +2780,7 @@
       <c r="V36" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="W36" s="17" t="s">
+      <c r="W36" s="16" t="s">
         <v>84</v>
       </c>
       <c r="X36" s="15"/>
@@ -2789,100 +2789,100 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="38"/>
-      <c r="P37" s="38"/>
-      <c r="Q37" s="38"/>
-      <c r="R37" s="38"/>
-      <c r="S37" s="38"/>
-      <c r="T37" s="38"/>
-      <c r="U37" s="38"/>
-      <c r="V37" s="38"/>
-      <c r="W37" s="38"/>
-      <c r="X37" s="38"/>
-      <c r="Y37" s="38"/>
-      <c r="Z37" s="39"/>
-    </row>
-    <row r="38" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="51"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="51"/>
+      <c r="R37" s="51"/>
+      <c r="S37" s="51"/>
+      <c r="T37" s="51"/>
+      <c r="U37" s="51"/>
+      <c r="V37" s="51"/>
+      <c r="W37" s="51"/>
+      <c r="X37" s="51"/>
+      <c r="Y37" s="51"/>
+      <c r="Z37" s="52"/>
+    </row>
+    <row r="38" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41"/>
-      <c r="M38" s="41"/>
-      <c r="N38" s="41"/>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="41"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="41"/>
-      <c r="V38" s="41"/>
-      <c r="W38" s="41"/>
-      <c r="X38" s="41"/>
-      <c r="Y38" s="41"/>
-      <c r="Z38" s="42"/>
-    </row>
-    <row r="39" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="54"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="54"/>
+      <c r="N38" s="54"/>
+      <c r="O38" s="54"/>
+      <c r="P38" s="54"/>
+      <c r="Q38" s="54"/>
+      <c r="R38" s="54"/>
+      <c r="S38" s="54"/>
+      <c r="T38" s="54"/>
+      <c r="U38" s="54"/>
+      <c r="V38" s="54"/>
+      <c r="W38" s="54"/>
+      <c r="X38" s="54"/>
+      <c r="Y38" s="54"/>
+      <c r="Z38" s="55"/>
+    </row>
+    <row r="39" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B39" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21"/>
-      <c r="R39" s="21"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-      <c r="V39" s="21"/>
-      <c r="W39" s="21"/>
-      <c r="X39" s="21"/>
-      <c r="Y39" s="21"/>
-      <c r="Z39" s="22"/>
-    </row>
-    <row r="40" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="40"/>
+      <c r="N39" s="40"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="40"/>
+      <c r="Q39" s="40"/>
+      <c r="R39" s="40"/>
+      <c r="S39" s="40"/>
+      <c r="T39" s="40"/>
+      <c r="U39" s="40"/>
+      <c r="V39" s="40"/>
+      <c r="W39" s="40"/>
+      <c r="X39" s="40"/>
+      <c r="Y39" s="40"/>
+      <c r="Z39" s="41"/>
+    </row>
+    <row r="40" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B40" s="8" t="s">
         <v>19</v>
       </c>
@@ -2913,116 +2913,95 @@
       <c r="Y40" s="18"/>
       <c r="Z40" s="14"/>
     </row>
-    <row r="41" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="21"/>
-      <c r="S41" s="21"/>
-      <c r="T41" s="21"/>
-      <c r="U41" s="21"/>
-      <c r="V41" s="21"/>
-      <c r="W41" s="21"/>
-      <c r="X41" s="21"/>
-      <c r="Y41" s="21"/>
-      <c r="Z41" s="22"/>
-    </row>
-    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C41" s="39"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="40"/>
+      <c r="N41" s="40"/>
+      <c r="O41" s="40"/>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="40"/>
+      <c r="R41" s="40"/>
+      <c r="S41" s="40"/>
+      <c r="T41" s="40"/>
+      <c r="U41" s="40"/>
+      <c r="V41" s="40"/>
+      <c r="W41" s="40"/>
+      <c r="X41" s="40"/>
+      <c r="Y41" s="40"/>
+      <c r="Z41" s="41"/>
+    </row>
+    <row r="42" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B42" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="23"/>
-      <c r="R42" s="23"/>
-      <c r="S42" s="23"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="23"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="23"/>
-      <c r="X42" s="23"/>
-      <c r="Y42" s="23"/>
-      <c r="Z42" s="24"/>
-    </row>
-    <row r="43" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="39"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="42"/>
+      <c r="Q42" s="42"/>
+      <c r="R42" s="42"/>
+      <c r="S42" s="42"/>
+      <c r="T42" s="42"/>
+      <c r="U42" s="42"/>
+      <c r="V42" s="42"/>
+      <c r="W42" s="42"/>
+      <c r="X42" s="42"/>
+      <c r="Y42" s="42"/>
+      <c r="Z42" s="43"/>
+    </row>
+    <row r="43" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="26"/>
-      <c r="L43" s="26"/>
-      <c r="M43" s="26"/>
-      <c r="N43" s="26"/>
-      <c r="O43" s="26"/>
-      <c r="P43" s="26"/>
-      <c r="Q43" s="26"/>
-      <c r="R43" s="26"/>
-      <c r="S43" s="26"/>
-      <c r="T43" s="26"/>
-      <c r="U43" s="26"/>
-      <c r="V43" s="26"/>
-      <c r="W43" s="26"/>
-      <c r="X43" s="26"/>
-      <c r="Y43" s="26"/>
-      <c r="Z43" s="27"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="45"/>
+      <c r="L43" s="45"/>
+      <c r="M43" s="45"/>
+      <c r="N43" s="45"/>
+      <c r="O43" s="45"/>
+      <c r="P43" s="45"/>
+      <c r="Q43" s="45"/>
+      <c r="R43" s="45"/>
+      <c r="S43" s="45"/>
+      <c r="T43" s="45"/>
+      <c r="U43" s="45"/>
+      <c r="V43" s="45"/>
+      <c r="W43" s="45"/>
+      <c r="X43" s="45"/>
+      <c r="Y43" s="45"/>
+      <c r="Z43" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="W3:W8"/>
-    <mergeCell ref="S3:S8"/>
-    <mergeCell ref="H3:H8"/>
-    <mergeCell ref="I3:I8"/>
-    <mergeCell ref="J3:J8"/>
-    <mergeCell ref="K3:K8"/>
-    <mergeCell ref="L3:L8"/>
-    <mergeCell ref="M3:M8"/>
-    <mergeCell ref="N3:N8"/>
-    <mergeCell ref="O3:O8"/>
-    <mergeCell ref="P3:P8"/>
-    <mergeCell ref="Q3:Q8"/>
-    <mergeCell ref="R3:R8"/>
-    <mergeCell ref="C1:Y1"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:T2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="X2:Y2"/>
     <mergeCell ref="C39:Z39"/>
     <mergeCell ref="C41:Z41"/>
     <mergeCell ref="C42:Z42"/>
@@ -3039,6 +3018,27 @@
     <mergeCell ref="E3:E8"/>
     <mergeCell ref="F3:F8"/>
     <mergeCell ref="G3:G8"/>
+    <mergeCell ref="C1:Y1"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:T2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="W3:W8"/>
+    <mergeCell ref="S3:S8"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="I3:I8"/>
+    <mergeCell ref="J3:J8"/>
+    <mergeCell ref="K3:K8"/>
+    <mergeCell ref="L3:L8"/>
+    <mergeCell ref="M3:M8"/>
+    <mergeCell ref="N3:N8"/>
+    <mergeCell ref="O3:O8"/>
+    <mergeCell ref="P3:P8"/>
+    <mergeCell ref="Q3:Q8"/>
+    <mergeCell ref="R3:R8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="76" orientation="landscape" r:id="rId1"/>
@@ -3056,295 +3056,295 @@
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="25" width="4.7109375" customWidth="1"/>
-    <col min="26" max="26" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="25" width="4.6640625" customWidth="1"/>
+    <col min="26" max="26" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="C1" s="49" t="s">
+    <row r="1" spans="2:26" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="C1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-    </row>
-    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+    </row>
+    <row r="2" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50" t="s">
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50" t="s">
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50" t="s">
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="50"/>
+      <c r="Y2" s="38"/>
       <c r="Z2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="52" t="s">
+      <c r="I3" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="31" t="s">
+      <c r="L3" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="M3" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="O3" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="P3" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="Q3" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="R3" s="46" t="s">
+      <c r="R3" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="S3" s="46" t="s">
+      <c r="S3" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="31" t="s">
+      <c r="T3" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="U3" s="28" t="s">
+      <c r="U3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="43" t="s">
+      <c r="V3" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="W3" s="31" t="s">
+      <c r="W3" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="X3" s="28" t="s">
+      <c r="X3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" s="31" t="s">
+      <c r="Y3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="Z3" s="34" t="s">
+      <c r="Z3" s="47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="51"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="44"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="35"/>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B5" s="51"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="47"/>
-      <c r="S5" s="47"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="32"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="35"/>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B6" s="51"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="44"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="35"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B7" s="51"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
-      <c r="S7" s="47"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="29"/>
-      <c r="V7" s="44"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="35"/>
-    </row>
-    <row r="8" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="51"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="33"/>
-      <c r="X8" s="30"/>
-      <c r="Y8" s="33"/>
-      <c r="Z8" s="36"/>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B4" s="24"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="26"/>
+      <c r="Z4" s="48"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B5" s="24"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="26"/>
+      <c r="Z5" s="48"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B6" s="24"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="35"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="48"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B7" s="24"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="48"/>
+    </row>
+    <row r="8" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="24"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="49"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
@@ -3373,7 +3373,7 @@
       <c r="Y9" s="19"/>
       <c r="Z9" s="4"/>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B11" s="12" t="s">
         <v>29</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
         <v>49</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
         <v>50</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
         <v>51</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
         <v>52</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>2</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
         <v>44</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
         <v>33</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B19" s="12" t="s">
         <v>47</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B20" s="12" t="s">
         <v>46</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
         <v>48</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>3</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
         <v>30</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B24" s="12" t="s">
         <v>31</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B25" s="12" t="s">
         <v>32</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B26" s="12" t="s">
         <v>34</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B27" s="12" t="s">
         <v>35</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
         <v>36</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B29" s="12" t="s">
         <v>37</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B30" s="12" t="s">
         <v>38</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
         <v>39</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="s">
         <v>40</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B33" s="12" t="s">
         <v>41</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B34" s="12" t="s">
         <v>42</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B35" s="12" t="s">
         <v>43</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B36" s="12" t="s">
         <v>45</v>
       </c>
@@ -4454,100 +4454,100 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="38"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="38"/>
-      <c r="P37" s="38"/>
-      <c r="Q37" s="38"/>
-      <c r="R37" s="38"/>
-      <c r="S37" s="38"/>
-      <c r="T37" s="38"/>
-      <c r="U37" s="38"/>
-      <c r="V37" s="38"/>
-      <c r="W37" s="38"/>
-      <c r="X37" s="38"/>
-      <c r="Y37" s="38"/>
-      <c r="Z37" s="39"/>
-    </row>
-    <row r="38" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="51"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="51"/>
+      <c r="R37" s="51"/>
+      <c r="S37" s="51"/>
+      <c r="T37" s="51"/>
+      <c r="U37" s="51"/>
+      <c r="V37" s="51"/>
+      <c r="W37" s="51"/>
+      <c r="X37" s="51"/>
+      <c r="Y37" s="51"/>
+      <c r="Z37" s="52"/>
+    </row>
+    <row r="38" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41"/>
-      <c r="M38" s="41"/>
-      <c r="N38" s="41"/>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="41"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="41"/>
-      <c r="V38" s="41"/>
-      <c r="W38" s="41"/>
-      <c r="X38" s="41"/>
-      <c r="Y38" s="41"/>
-      <c r="Z38" s="42"/>
-    </row>
-    <row r="39" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="54"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="54"/>
+      <c r="N38" s="54"/>
+      <c r="O38" s="54"/>
+      <c r="P38" s="54"/>
+      <c r="Q38" s="54"/>
+      <c r="R38" s="54"/>
+      <c r="S38" s="54"/>
+      <c r="T38" s="54"/>
+      <c r="U38" s="54"/>
+      <c r="V38" s="54"/>
+      <c r="W38" s="54"/>
+      <c r="X38" s="54"/>
+      <c r="Y38" s="54"/>
+      <c r="Z38" s="55"/>
+    </row>
+    <row r="39" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B39" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="21"/>
-      <c r="P39" s="21"/>
-      <c r="Q39" s="21"/>
-      <c r="R39" s="21"/>
-      <c r="S39" s="21"/>
-      <c r="T39" s="21"/>
-      <c r="U39" s="21"/>
-      <c r="V39" s="21"/>
-      <c r="W39" s="21"/>
-      <c r="X39" s="21"/>
-      <c r="Y39" s="21"/>
-      <c r="Z39" s="22"/>
-    </row>
-    <row r="40" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="40"/>
+      <c r="N39" s="40"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="40"/>
+      <c r="Q39" s="40"/>
+      <c r="R39" s="40"/>
+      <c r="S39" s="40"/>
+      <c r="T39" s="40"/>
+      <c r="U39" s="40"/>
+      <c r="V39" s="40"/>
+      <c r="W39" s="40"/>
+      <c r="X39" s="40"/>
+      <c r="Y39" s="40"/>
+      <c r="Z39" s="41"/>
+    </row>
+    <row r="40" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B40" s="8" t="s">
         <v>19</v>
       </c>
@@ -4578,111 +4578,100 @@
       <c r="Y40" s="18"/>
       <c r="Z40" s="14"/>
     </row>
-    <row r="41" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21"/>
-      <c r="O41" s="21"/>
-      <c r="P41" s="21"/>
-      <c r="Q41" s="21"/>
-      <c r="R41" s="21"/>
-      <c r="S41" s="21"/>
-      <c r="T41" s="21"/>
-      <c r="U41" s="21"/>
-      <c r="V41" s="21"/>
-      <c r="W41" s="21"/>
-      <c r="X41" s="21"/>
-      <c r="Y41" s="21"/>
-      <c r="Z41" s="22"/>
-    </row>
-    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="C41" s="39"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="40"/>
+      <c r="N41" s="40"/>
+      <c r="O41" s="40"/>
+      <c r="P41" s="40"/>
+      <c r="Q41" s="40"/>
+      <c r="R41" s="40"/>
+      <c r="S41" s="40"/>
+      <c r="T41" s="40"/>
+      <c r="U41" s="40"/>
+      <c r="V41" s="40"/>
+      <c r="W41" s="40"/>
+      <c r="X41" s="40"/>
+      <c r="Y41" s="40"/>
+      <c r="Z41" s="41"/>
+    </row>
+    <row r="42" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B42" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="23"/>
-      <c r="R42" s="23"/>
-      <c r="S42" s="23"/>
-      <c r="T42" s="23"/>
-      <c r="U42" s="23"/>
-      <c r="V42" s="23"/>
-      <c r="W42" s="23"/>
-      <c r="X42" s="23"/>
-      <c r="Y42" s="23"/>
-      <c r="Z42" s="24"/>
-    </row>
-    <row r="43" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="39"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="42"/>
+      <c r="Q42" s="42"/>
+      <c r="R42" s="42"/>
+      <c r="S42" s="42"/>
+      <c r="T42" s="42"/>
+      <c r="U42" s="42"/>
+      <c r="V42" s="42"/>
+      <c r="W42" s="42"/>
+      <c r="X42" s="42"/>
+      <c r="Y42" s="42"/>
+      <c r="Z42" s="43"/>
+    </row>
+    <row r="43" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="26"/>
-      <c r="L43" s="26"/>
-      <c r="M43" s="26"/>
-      <c r="N43" s="26"/>
-      <c r="O43" s="26"/>
-      <c r="P43" s="26"/>
-      <c r="Q43" s="26"/>
-      <c r="R43" s="26"/>
-      <c r="S43" s="26"/>
-      <c r="T43" s="26"/>
-      <c r="U43" s="26"/>
-      <c r="V43" s="26"/>
-      <c r="W43" s="26"/>
-      <c r="X43" s="26"/>
-      <c r="Y43" s="26"/>
-      <c r="Z43" s="27"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="45"/>
+      <c r="L43" s="45"/>
+      <c r="M43" s="45"/>
+      <c r="N43" s="45"/>
+      <c r="O43" s="45"/>
+      <c r="P43" s="45"/>
+      <c r="Q43" s="45"/>
+      <c r="R43" s="45"/>
+      <c r="S43" s="45"/>
+      <c r="T43" s="45"/>
+      <c r="U43" s="45"/>
+      <c r="V43" s="45"/>
+      <c r="W43" s="45"/>
+      <c r="X43" s="45"/>
+      <c r="Y43" s="45"/>
+      <c r="Z43" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="I3:I8"/>
-    <mergeCell ref="K3:K8"/>
-    <mergeCell ref="L3:L8"/>
-    <mergeCell ref="M3:M8"/>
-    <mergeCell ref="F3:F8"/>
-    <mergeCell ref="G3:G8"/>
-    <mergeCell ref="H3:H8"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:T2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="S3:S8"/>
+    <mergeCell ref="O3:O8"/>
+    <mergeCell ref="P3:P8"/>
+    <mergeCell ref="Q3:Q8"/>
+    <mergeCell ref="R3:R8"/>
     <mergeCell ref="C42:Z42"/>
     <mergeCell ref="C43:Z43"/>
     <mergeCell ref="C1:Y1"/>
@@ -4699,11 +4688,22 @@
     <mergeCell ref="J3:J8"/>
     <mergeCell ref="X3:X8"/>
     <mergeCell ref="Y3:Y8"/>
-    <mergeCell ref="S3:S8"/>
-    <mergeCell ref="O3:O8"/>
-    <mergeCell ref="P3:P8"/>
-    <mergeCell ref="Q3:Q8"/>
-    <mergeCell ref="R3:R8"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:T2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="K3:K8"/>
+    <mergeCell ref="L3:L8"/>
+    <mergeCell ref="M3:M8"/>
+    <mergeCell ref="F3:F8"/>
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="I3:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="76" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
@@ -4711,6 +4711,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B2329572E014494A95DF6ACDEF2AB807" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="10fbc389776b026f7c16e416a9a098d0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="7257a348-19a8-418f-9646-fda164151095" xmlns:ns4="2afdcc8b-7dbd-467f-adcb-446ee327e55e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3db26c0c3e309abb292ab8e87594ec91" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4950,25 +4968,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{091A2A7A-E484-4B78-9C83-FFBBB8521EAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7257a348-19a8-418f-9646-fda164151095"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2afdcc8b-7dbd-467f-adcb-446ee327e55e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2206B09-11B3-4CA1-9BF6-983518461739}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CEB81878-6A5E-423F-8947-46D09B91C0E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4986,30 +5012,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2206B09-11B3-4CA1-9BF6-983518461739}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{091A2A7A-E484-4B78-9C83-FFBBB8521EAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7257a348-19a8-418f-9646-fda164151095"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2afdcc8b-7dbd-467f-adcb-446ee327e55e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>